<commit_message>
features: https; 部署到 阿里云
</commit_message>
<xml_diff>
--- a/server/files/result.xlsx
+++ b/server/files/result.xlsx
@@ -387,7 +387,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
@@ -417,7 +417,7 @@
         <v>3.019</v>
       </c>
       <c r="B2" s="2" t="str">
-        <v>1.479</v>
+        <v>1.480</v>
       </c>
       <c r="C2" s="2" t="str">
         <v>4.014</v>
@@ -426,10 +426,10 @@
         <v>35.447</v>
       </c>
       <c r="E2" s="2" t="str">
-        <v>13.736</v>
+        <v>12.579</v>
       </c>
       <c r="F2" s="2" t="str">
-        <v>6.301 %</v>
+        <v>5.547 %</v>
       </c>
     </row>
     <row r="3">
@@ -449,7 +449,7 @@
         <v>12.753</v>
       </c>
       <c r="F3" s="2" t="str">
-        <v>5.850 %</v>
+        <v>5.624 %</v>
       </c>
     </row>
     <row r="4">
@@ -469,12 +469,12 @@
         <v>13.262</v>
       </c>
       <c r="F4" s="2" t="str">
-        <v>6.084 %</v>
+        <v>5.848 %</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="str">
-        <v>7.098</v>
+        <v>7.099</v>
       </c>
       <c r="B5" s="2" t="str">
         <v>6.408</v>
@@ -483,13 +483,13 @@
         <v>8.169</v>
       </c>
       <c r="D5" s="2" t="str">
-        <v>34.339</v>
+        <v>34.332</v>
       </c>
       <c r="E5" s="2" t="str">
-        <v>12.797</v>
+        <v>10.464</v>
       </c>
       <c r="F5" s="2" t="str">
-        <v>5.871 %</v>
+        <v>4.614 %</v>
       </c>
     </row>
     <row r="6">
@@ -500,16 +500,16 @@
         <v>8.170</v>
       </c>
       <c r="C6" s="2" t="str">
-        <v>10.117</v>
+        <v>10.137</v>
       </c>
       <c r="D6" s="2" t="str">
         <v>19.691</v>
       </c>
       <c r="E6" s="2" t="str">
-        <v>3.599</v>
+        <v>2.509</v>
       </c>
       <c r="F6" s="2" t="str">
-        <v>1.651 %</v>
+        <v>1.106 %</v>
       </c>
     </row>
     <row r="7">
@@ -520,16 +520,16 @@
         <v>11.261</v>
       </c>
       <c r="C7" s="2" t="str">
-        <v>13.188</v>
+        <v>13.062</v>
       </c>
       <c r="D7" s="2" t="str">
         <v>47.034</v>
       </c>
       <c r="E7" s="2" t="str">
-        <v>24.739</v>
+        <v>24.016</v>
       </c>
       <c r="F7" s="2" t="str">
-        <v>11.349 %</v>
+        <v>10.591 %</v>
       </c>
     </row>
     <row r="8">
@@ -537,19 +537,19 @@
         <v>13.571</v>
       </c>
       <c r="B8" s="2" t="str">
-        <v>13.188</v>
+        <v>13.172</v>
       </c>
       <c r="C8" s="2" t="str">
-        <v>15.123</v>
+        <v>15.122</v>
       </c>
       <c r="D8" s="2" t="str">
         <v>28.592</v>
       </c>
       <c r="E8" s="2" t="str">
-        <v>9.831</v>
+        <v>9.952</v>
       </c>
       <c r="F8" s="2" t="str">
-        <v>4.510 %</v>
+        <v>4.389 %</v>
       </c>
     </row>
     <row r="9">
@@ -557,19 +557,19 @@
         <v>17.019</v>
       </c>
       <c r="B9" s="2" t="str">
-        <v>15.262</v>
+        <v>15.261</v>
       </c>
       <c r="C9" s="2" t="str">
-        <v>18.045</v>
+        <v>18.188</v>
       </c>
       <c r="D9" s="2" t="str">
         <v>28.967</v>
       </c>
       <c r="E9" s="2" t="str">
-        <v>15.710</v>
+        <v>14.765</v>
       </c>
       <c r="F9" s="2" t="str">
-        <v>7.207 %</v>
+        <v>6.511 %</v>
       </c>
     </row>
     <row r="10">
@@ -577,7 +577,7 @@
         <v>18.859</v>
       </c>
       <c r="B10" s="2" t="str">
-        <v>18.046</v>
+        <v>18.188</v>
       </c>
       <c r="C10" s="2" t="str">
         <v>21.733</v>
@@ -586,10 +586,10 @@
         <v>24.353</v>
       </c>
       <c r="E10" s="2" t="str">
-        <v>12.072</v>
+        <v>10.056</v>
       </c>
       <c r="F10" s="2" t="str">
-        <v>5.538 %</v>
+        <v>4.435 %</v>
       </c>
     </row>
     <row r="11">
@@ -606,10 +606,10 @@
         <v>42.163</v>
       </c>
       <c r="E11" s="2" t="str">
-        <v>18.346</v>
+        <v>16.755</v>
       </c>
       <c r="F11" s="2" t="str">
-        <v>8.416 %</v>
+        <v>7.389 %</v>
       </c>
     </row>
     <row r="12">
@@ -620,36 +620,36 @@
         <v>23.670</v>
       </c>
       <c r="C12" s="2" t="str">
-        <v>25.122</v>
+        <v>25.017</v>
       </c>
       <c r="D12" s="2" t="str">
         <v>29.934</v>
       </c>
       <c r="E12" s="2" t="str">
-        <v>11.506</v>
+        <v>10.345</v>
       </c>
       <c r="F12" s="2" t="str">
-        <v>5.278 %</v>
+        <v>4.562 %</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="str">
-        <v>25.455</v>
+        <v>25.456</v>
       </c>
       <c r="B13" s="2" t="str">
-        <v>25.123</v>
+        <v>25.018</v>
       </c>
       <c r="C13" s="2" t="str">
         <v>26.965</v>
       </c>
       <c r="D13" s="2" t="str">
-        <v>36.535</v>
+        <v>36.526</v>
       </c>
       <c r="E13" s="2" t="str">
-        <v>14.583</v>
+        <v>13.218</v>
       </c>
       <c r="F13" s="2" t="str">
-        <v>6.690 %</v>
+        <v>5.829 %</v>
       </c>
     </row>
     <row r="14">
@@ -666,10 +666,10 @@
         <v>35.488</v>
       </c>
       <c r="E14" s="2" t="str">
-        <v>20.100</v>
+        <v>18.811</v>
       </c>
       <c r="F14" s="2" t="str">
-        <v>9.221 %</v>
+        <v>8.295 %</v>
       </c>
     </row>
     <row r="15">
@@ -686,15 +686,15 @@
         <v>32.315</v>
       </c>
       <c r="E15" s="2" t="str">
-        <v>17.433</v>
+        <v>15.613</v>
       </c>
       <c r="F15" s="2" t="str">
-        <v>7.997 %</v>
+        <v>6.885 %</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="str">
-        <v>40.267</v>
+        <v>40.301</v>
       </c>
       <c r="B16" s="2" t="str">
         <v>38.868</v>
@@ -703,13 +703,33 @@
         <v>41.388</v>
       </c>
       <c r="D16" s="2" t="str">
-        <v>32.923</v>
+        <v>32.976</v>
       </c>
       <c r="E16" s="2" t="str">
-        <v>17.517</v>
+        <v>15.123</v>
       </c>
       <c r="F16" s="2" t="str">
-        <v>8.036 %</v>
+        <v>6.669 %</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="str">
+        <v>42.314</v>
+      </c>
+      <c r="B17" s="2" t="str">
+        <v>41.389</v>
+      </c>
+      <c r="C17" s="2" t="str">
+        <v>44.928</v>
+      </c>
+      <c r="D17" s="2" t="str">
+        <v>40.537</v>
+      </c>
+      <c r="E17" s="2" t="str">
+        <v>26.546</v>
+      </c>
+      <c r="F17" s="2" t="str">
+        <v>11.706 %</v>
       </c>
     </row>
   </sheetData>

</xml_diff>